<commit_message>
Windows Rebuild (Update 08-03-2017)
</commit_message>
<xml_diff>
--- a/release-builds/Buildability Certifier-win32-ia32/resources/app/userdata-backups/10.xlsx
+++ b/release-builds/Buildability Certifier-win32-ia32/resources/app/userdata-backups/10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="608">
   <si>
     <t>Name</t>
   </si>
@@ -52,10 +52,10 @@
     <t>0001</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>steven.xie@outlook.com</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>0002</t>
@@ -2232,22 +2232,25 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
       <c r="F2" t="str">
         <f>TEXT(ROW(C1),"0000")</f>
         <v>0001</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="str">
         <f>TEXT(ROW(E1),"0000")</f>
         <v>0001</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="1">"Frederick J. Boyd (" &amp; F3 &amp; ")"</f>
         <v>Frederick J. Boyd (0002)</v>
@@ -2261,19 +2264,25 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:H66" si="0">TEXT(ROW(C2),"0000")</f>
         <v>0002</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
         <v>0002</v>
       </c>
-    </row>
-    <row r="4" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0003)</v>
@@ -2287,19 +2296,25 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>0003</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>0003</v>
       </c>
-    </row>
-    <row r="5" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0004)</v>
@@ -2318,14 +2333,17 @@
         <v>0004</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>0004</v>
       </c>
-    </row>
-    <row r="6" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0005)</v>
@@ -2344,14 +2362,17 @@
         <v>0005</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>0005</v>
       </c>
-    </row>
-    <row r="7" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0006)</v>
@@ -2370,14 +2391,17 @@
         <v>0006</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>0006</v>
       </c>
-    </row>
-    <row r="8" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0007)</v>
@@ -2396,14 +2420,17 @@
         <v>0007</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>0007</v>
       </c>
-    </row>
-    <row r="9" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0008)</v>
@@ -2422,14 +2449,17 @@
         <v>0008</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>0008</v>
       </c>
-    </row>
-    <row r="10" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0009)</v>
@@ -2448,14 +2478,17 @@
         <v>0009</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>0009</v>
       </c>
-    </row>
-    <row r="11" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0010)</v>
@@ -2474,14 +2507,17 @@
         <v>0010</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>0010</v>
       </c>
-    </row>
-    <row r="12" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0011)</v>
@@ -2500,14 +2536,17 @@
         <v>0011</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>0011</v>
       </c>
-    </row>
-    <row r="13" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0012)</v>
@@ -2526,14 +2565,17 @@
         <v>0012</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>0012</v>
       </c>
-    </row>
-    <row r="14" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0013)</v>
@@ -2552,11 +2594,14 @@
         <v>0013</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>0013</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2578,14 +2623,14 @@
         <v>0014</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>0014</v>
       </c>
     </row>
-    <row r="16" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0015)</v>
@@ -2604,11 +2649,14 @@
         <v>0015</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>0015</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2630,7 +2678,7 @@
         <v>0016</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -2656,7 +2704,7 @@
         <v>0017</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -2682,7 +2730,7 @@
         <v>0018</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -2708,7 +2756,7 @@
         <v>0019</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -2734,7 +2782,7 @@
         <v>0020</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>

</xml_diff>